<commit_message>
[0.0.2] - 2025-06-09 Beginning As Built Documentation
</commit_message>
<xml_diff>
--- a/Video_Sound/Overview_Notes.xlsx
+++ b/Video_Sound/Overview_Notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/99d2d0efc5e421e1/Working Files/CPC_Production/Video_Sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="11_F25DC773A252ABDACC1048B0395B70645BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4304E2D-1A70-4CBB-92B2-B827E9AC0A1D}"/>
+  <xr:revisionPtr revIDLastSave="195" documentId="11_F25DC773A252ABDACC1048B0395B70645BDE58E6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D098B1AA-C27E-40E8-943E-423E60B2BFD5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -31,18 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="59">
   <si>
     <t>Device</t>
-  </si>
-  <si>
-    <t>Roles</t>
-  </si>
-  <si>
-    <t>Connection Type</t>
-  </si>
-  <si>
-    <t>Logical Flow</t>
   </si>
   <si>
     <t>Board</t>
@@ -62,9 +53,6 @@
   <si>
     <t>IN:
 OUT:</t>
-  </si>
-  <si>
-    <t>Process Source Audio, route to house speakers and amps, route to video</t>
   </si>
   <si>
     <t>Process Video and Audio into standard format for streaming</t>
@@ -253,12 +241,98 @@
   <si>
     <t>Other?</t>
   </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>Outputs</t>
+  </si>
+  <si>
+    <t>Roles (e.g., FOH Mix, Stream Audio, Confidence Monitor)</t>
+  </si>
+  <si>
+    <t>Connection types (HDMI, SDI, XLR, USB, Dante, NDI, etc.)</t>
+  </si>
+  <si>
+    <t>Logical Flow (Source → Processor → Output)</t>
+  </si>
+  <si>
+    <t>Process Source Audio to generate FOH Mix and Stream Audio</t>
+  </si>
+  <si>
+    <t>Behringer X32</t>
+  </si>
+  <si>
+    <t>Radial J-ISO Stereo Isolator</t>
+  </si>
+  <si>
+    <t>Isolator -- NOT USED</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">IN  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>???</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+OUT:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ???</t>
+    </r>
+  </si>
+  <si>
+    <t>URayCoder 
+USE265-1L</t>
+  </si>
+  <si>
+    <t>Video / Audio Mix:  SDI From Switcher
+Control/Config:  Ethernet</t>
+  </si>
+  <si>
+    <t>Stream:  Ethernet to Internet</t>
+  </si>
+  <si>
+    <t>Black Magic Model???</t>
+  </si>
+  <si>
+    <t>Video:  HDMI from Cameras
+Audio:  Balanced Line from Board</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,6 +350,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -318,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -338,6 +419,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,6 +715,59 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1251172</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>146190</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47474E2A-2958-FB50-8A8E-65F6F914C02E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2146300" y="6813550"/>
+          <a:ext cx="4324572" cy="2724290"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -903,130 +1046,186 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{314C194A-741B-42BF-8957-20D85777A846}">
-  <dimension ref="B2:E11"/>
+  <dimension ref="B2:H11"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="22" customWidth="1"/>
-    <col min="3" max="3" width="26.6328125" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" customWidth="1"/>
-    <col min="5" max="5" width="40.7265625" customWidth="1"/>
+    <col min="1" max="1" width="3.7265625" customWidth="1"/>
+    <col min="2" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="26.6328125" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" customWidth="1"/>
+    <col min="8" max="8" width="40.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.35">
-      <c r="B2" t="s">
+    <row r="2" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="2:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="2:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="2:8" ht="58" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="2:5" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="2:8" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="2:5" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="2:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>9</v>
+      <c r="G11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1037,7 +1236,7 @@
   </sheetPr>
   <dimension ref="B1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
@@ -1051,127 +1250,127 @@
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="2:7" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="F4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="2:7" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="2:7" ht="105" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="5" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>

</xml_diff>